<commit_message>
Just making sure everything is updated
</commit_message>
<xml_diff>
--- a/Documentation/Final Checklist.xlsx
+++ b/Documentation/Final Checklist.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Desktop\INFO 340\Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\PatientAppointmentDB\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22650" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22650" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -630,7 +630,7 @@
   <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J10:J11"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +721,7 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
         <v>19</v>
@@ -739,7 +739,7 @@
         <v>2</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="G6" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Exec and roll back and commit
</commit_message>
<xml_diff>
--- a/Documentation/Final Checklist.xlsx
+++ b/Documentation/Final Checklist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22650" windowHeight="7830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22656" windowHeight="7836"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,28 +73,6 @@
         <rFont val="Times New Roman"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>An ERD</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <charset val="1"/>
-      </rPr>
       <t xml:space="preserve"> </t>
     </r>
     <r>
@@ -157,6 +135,28 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>An ERD</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -630,22 +630,22 @@
   <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:10" ht="21" x14ac:dyDescent="0.4">
       <c r="B1" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -656,7 +656,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
@@ -673,7 +673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="6">
         <v>5</v>
       </c>
@@ -688,16 +688,16 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="6">
         <v>50</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E4">
         <v>0.5</v>
@@ -706,34 +706,34 @@
         <v>0.5</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="6">
         <v>5</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="6">
         <v>50</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -742,16 +742,16 @@
         <v>4.5</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="6">
         <v>5</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -760,16 +760,16 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="6">
         <v>100</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <v>0.5</v>
@@ -778,46 +778,55 @@
         <v>0.5</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="6">
         <v>100</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="6">
         <v>5</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="6">
         <v>100</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="6">
         <v>100</v>
       </c>
@@ -828,8 +837,11 @@
       <c r="E12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <f>SUM(B3:B12)</f>
         <v>520</v>
@@ -845,17 +857,19 @@
         <f>SUM(E3:E12)</f>
         <v>16</v>
       </c>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F13" s="5">
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
       <c r="C14" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -873,7 +887,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -885,7 +899,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>